<commit_message>
kong commit Ai model
</commit_message>
<xml_diff>
--- a/kong/Diw/data/ModelGas.xlsx
+++ b/kong/Diw/data/ModelGas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kong0\Desktop\AI_Fac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kong0\Desktop\AI\kong\Diw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D720DC-512E-44B3-A66D-31C217FE762F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA7EA12-5EBB-4B8A-B52B-31DCE30EA99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{4ABA209E-1626-4583-9C2C-17BC4E1318E1}"/>
+    <workbookView minimized="1" xWindow="43305" yWindow="2580" windowWidth="23205" windowHeight="11235" xr2:uid="{4ABA209E-1626-4583-9C2C-17BC4E1318E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -683,14 +683,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6919458-6032-4CBC-B52D-025732B172CF}">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="32.296875" customWidth="1"/>
-    <col min="2" max="2" width="62.796875" customWidth="1"/>
+    <col min="2" max="2" width="88.8984375" customWidth="1"/>
     <col min="3" max="3" width="23.69921875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1373,6 +1373,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="เอกสาร" ma:contentTypeID="0x0101008FD3405EC0999D4390A05CC445851E56" ma:contentTypeVersion="15" ma:contentTypeDescription="สร้างเอกสารใหม่" ma:contentTypeScope="" ma:versionID="cff76b32ab010cb70be918a74d1bb730">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ffb6699a-b691-46f2-86b8-8c6f27c7e174" xmlns:ns4="3c9a746d-86cc-4690-a5a0-dd6ba556647c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eefe135cfa4fb2fc944f55112e4e48e5" ns3:_="" ns4:_="">
     <xsd:import namespace="ffb6699a-b691-46f2-86b8-8c6f27c7e174"/>
@@ -1605,15 +1614,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1623,6 +1623,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F10A6414-6971-4B02-B949-7F91784A1168}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BBEF2DD-3A33-491C-894B-B7EB4119FEEB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1637,14 +1645,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F10A6414-6971-4B02-B949-7F91784A1168}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>